<commit_message>
Add maps of density trends at sites
</commit_message>
<xml_diff>
--- a/raw_data/Temps de génération.xlsx
+++ b/raw_data/Temps de génération.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pascal.irz\Documents\projets\ASPE\liste_rouge_regionale\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F676FA07-5459-4744-9995-B6E560CA70D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350F03C4-8F8F-4247-B414-23C50E2C3945}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15090" windowHeight="5340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -567,7 +567,7 @@
   <dimension ref="A1:K993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -731,7 +731,7 @@
         <v>28</v>
       </c>
       <c r="F5" s="5">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="G5" s="5">
         <v>10</v>

</xml_diff>